<commit_message>
added 1802 in CR_210_2 as ed3, was in CR_itemshape_1 also as ed 2 - Bug 6266
</commit_message>
<xml_diff>
--- a/config_management/change_requests/modulesCR11.xlsx
+++ b/config_management/change_requests/modulesCR11.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-4080" yWindow="-21160" windowWidth="33600" windowHeight="20480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-6440" yWindow="-21160" windowWidth="38400" windowHeight="21160" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="10" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="CR_210-2 (2)" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Master CRs listing'!$A$1:$Q$206</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Master CRs listing'!$A$1:$Q$207</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2765" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2769" uniqueCount="329">
   <si>
     <t>Part number</t>
   </si>
@@ -1499,7 +1499,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1741,6 +1741,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="86">
@@ -11462,8 +11465,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:Q206" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
-  <autoFilter ref="A1:Q206"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:Q207" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <autoFilter ref="A1:Q207"/>
   <sortState ref="A2:Q206">
     <sortCondition ref="A1:A206"/>
   </sortState>
@@ -13343,13 +13346,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y206"/>
+  <dimension ref="A1:Y207"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B110" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B192" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D121" sqref="D121"/>
+      <selection pane="bottomRight" activeCell="D206" sqref="D206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -13362,14 +13365,15 @@
     <col min="6" max="6" width="19.1640625" style="28" customWidth="1"/>
     <col min="7" max="7" width="35.5" style="8" customWidth="1"/>
     <col min="8" max="8" width="19" style="44" customWidth="1"/>
-    <col min="9" max="10" width="10.83203125" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="15.1640625" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="14.33203125" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="15" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="20" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="17.33203125" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="18" style="3" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="10.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="10" width="10.83203125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="15.1640625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="14.33203125" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="15" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="20" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="17.33203125" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="18" style="3" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="10.83203125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="10.83203125" collapsed="1"/>
     <col min="20" max="20" width="13.33203125" style="5" customWidth="1" outlineLevel="1"/>
     <col min="21" max="21" width="10.83203125" customWidth="1" outlineLevel="1"/>
     <col min="22" max="23" width="13.83203125" style="3" customWidth="1" outlineLevel="1"/>
@@ -21667,16 +21671,16 @@
       <c r="L145" s="17"/>
       <c r="M145" s="17"/>
       <c r="N145" s="18">
-        <f t="shared" ref="N145:N177" si="25">IF(ISBLANK(E145),0,1)</f>
+        <f t="shared" ref="N145:N178" si="25">IF(ISBLANK(E145),0,1)</f>
         <v>1</v>
       </c>
       <c r="O145" s="16"/>
       <c r="P145" s="18">
-        <f t="shared" ref="P145:P177" si="26">IF(ISBLANK(O145),IF(ISBLANK(E145),0,1),1)</f>
+        <f t="shared" ref="P145:P178" si="26">IF(ISBLANK(O145),IF(ISBLANK(E145),0,1),1)</f>
         <v>1</v>
       </c>
       <c r="Q145" s="19">
-        <f t="shared" ref="Q145:Q177" si="27">IF(AND(I145="Yes",J145="CR11",K145=L145,L145=M145,M145=E145),1,IF(AND(I145="Yes",J145="CR11",K145=M145,M145=E145),0.5,0))</f>
+        <f t="shared" ref="Q145:Q178" si="27">IF(AND(I145="Yes",J145="CR11",K145=L145,L145=M145,M145=E145),1,IF(AND(I145="Yes",J145="CR11",K145=M145,M145=E145),0.5,0))</f>
         <v>0</v>
       </c>
       <c r="R145" s="3"/>
@@ -23409,58 +23413,37 @@
     </row>
     <row r="175" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A175" s="98">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="B175" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="C175" s="54">
+        <v>216</v>
+      </c>
+      <c r="C175" s="36">
         <v>3</v>
       </c>
-      <c r="D175" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="E175" s="87" t="s">
-        <v>24</v>
-      </c>
-      <c r="F175" s="72" t="s">
+      <c r="D175" s="87" t="s">
+        <v>79</v>
+      </c>
+      <c r="E175" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="F175" s="71" t="s">
         <v>320</v>
       </c>
-      <c r="G175" s="20"/>
-      <c r="H175" s="65">
+      <c r="G175" s="72"/>
+      <c r="H175" s="102">
         <f>IF(Table2[[#This Row],[STEPmod publication index]]=Table2[[#This Row],[Final Listing]],1,0)</f>
         <v>1</v>
       </c>
-      <c r="I175" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J175" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="K175" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="L175" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="M175" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="N175" s="18">
-        <f t="shared" si="25"/>
-        <v>1</v>
-      </c>
-      <c r="O175" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="P175" s="18">
-        <f t="shared" si="26"/>
-        <v>1</v>
-      </c>
-      <c r="Q175" s="19">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
+      <c r="I175" s="16"/>
+      <c r="J175" s="16"/>
+      <c r="K175" s="37"/>
+      <c r="L175" s="16"/>
+      <c r="M175" s="17"/>
+      <c r="N175" s="18"/>
+      <c r="O175" s="16"/>
+      <c r="P175" s="18"/>
+      <c r="Q175" s="19"/>
       <c r="R175" s="3"/>
       <c r="S175" s="3"/>
       <c r="T175" s="3"/>
@@ -23470,18 +23453,18 @@
     </row>
     <row r="176" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A176" s="98">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="B176" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C176" s="54">
-        <v>2</v>
-      </c>
-      <c r="D176" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D176" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E176" s="31" t="s">
+      <c r="E176" s="87" t="s">
         <v>24</v>
       </c>
       <c r="F176" s="72" t="s">
@@ -23501,7 +23484,7 @@
       <c r="K176" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="L176" s="17" t="s">
+      <c r="L176" s="16" t="s">
         <v>24</v>
       </c>
       <c r="M176" s="21" t="s">
@@ -23531,10 +23514,10 @@
     </row>
     <row r="177" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A177" s="98">
-        <v>1806</v>
+        <v>1804</v>
       </c>
       <c r="B177" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C177" s="54">
         <v>2</v>
@@ -23545,7 +23528,7 @@
       <c r="E177" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="F177" s="87" t="s">
+      <c r="F177" s="72" t="s">
         <v>320</v>
       </c>
       <c r="G177" s="20"/>
@@ -23592,37 +23575,58 @@
     </row>
     <row r="178" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A178" s="98">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="B178" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="C178" s="36">
+        <v>219</v>
+      </c>
+      <c r="C178" s="54">
         <v>2</v>
       </c>
       <c r="D178" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="E178" s="53" t="s">
-        <v>29</v>
-      </c>
-      <c r="F178" s="71" t="s">
-        <v>322</v>
-      </c>
-      <c r="G178" s="72"/>
+        <v>24</v>
+      </c>
+      <c r="E178" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="F178" s="87" t="s">
+        <v>320</v>
+      </c>
+      <c r="G178" s="20"/>
       <c r="H178" s="65">
         <f>IF(Table2[[#This Row],[STEPmod publication index]]=Table2[[#This Row],[Final Listing]],1,0)</f>
         <v>1</v>
       </c>
-      <c r="I178" s="16"/>
-      <c r="J178" s="16"/>
-      <c r="K178" s="37"/>
-      <c r="L178" s="16"/>
-      <c r="M178" s="21"/>
-      <c r="N178" s="18"/>
-      <c r="O178" s="17"/>
-      <c r="P178" s="18"/>
-      <c r="Q178" s="19"/>
+      <c r="I178" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J178" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="K178" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="L178" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M178" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="N178" s="18">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="O178" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="P178" s="18">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="Q178" s="19">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
       <c r="R178" s="3"/>
       <c r="S178" s="3"/>
       <c r="T178" s="3"/>
@@ -23638,52 +23642,31 @@
         <v>220</v>
       </c>
       <c r="C179" s="36">
-        <v>3</v>
-      </c>
-      <c r="D179" s="56" t="s">
-        <v>38</v>
+        <v>2</v>
+      </c>
+      <c r="D179" s="31" t="s">
+        <v>29</v>
       </c>
       <c r="E179" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F179" s="72" t="s">
-        <v>321</v>
-      </c>
-      <c r="G179" s="20" t="s">
-        <v>317</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F179" s="71" t="s">
+        <v>322</v>
+      </c>
+      <c r="G179" s="72"/>
       <c r="H179" s="65">
         <f>IF(Table2[[#This Row],[STEPmod publication index]]=Table2[[#This Row],[Final Listing]],1,0)</f>
         <v>1</v>
       </c>
-      <c r="I179" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J179" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="K179" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="L179" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="M179" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="N179" s="18">
-        <f t="shared" ref="N179:N187" si="28">IF(ISBLANK(E179),0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="O179" s="16"/>
-      <c r="P179" s="18">
-        <f>IF(ISBLANK(O179),IF(ISBLANK(E179),0,1),1)</f>
-        <v>1</v>
-      </c>
-      <c r="Q179" s="19">
-        <f t="shared" ref="Q179:Q187" si="29">IF(AND(I179="Yes",J179="CR11",K179=L179,L179=M179,M179=E179),1,IF(AND(I179="Yes",J179="CR11",K179=M179,M179=E179),0.5,0))</f>
-        <v>0</v>
-      </c>
+      <c r="I179" s="16"/>
+      <c r="J179" s="16"/>
+      <c r="K179" s="37"/>
+      <c r="L179" s="16"/>
+      <c r="M179" s="21"/>
+      <c r="N179" s="18"/>
+      <c r="O179" s="17"/>
+      <c r="P179" s="18"/>
+      <c r="Q179" s="19"/>
       <c r="R179" s="3"/>
       <c r="S179" s="3"/>
       <c r="T179" s="3"/>
@@ -23693,24 +23676,26 @@
     </row>
     <row r="180" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A180" s="98">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="B180" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="C180" s="54">
-        <v>2</v>
-      </c>
-      <c r="D180" s="31" t="s">
-        <v>27</v>
+        <v>220</v>
+      </c>
+      <c r="C180" s="36">
+        <v>3</v>
+      </c>
+      <c r="D180" s="56" t="s">
+        <v>38</v>
       </c>
       <c r="E180" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="F180" s="71" t="s">
-        <v>323</v>
-      </c>
-      <c r="G180" s="72"/>
+        <v>38</v>
+      </c>
+      <c r="F180" s="72" t="s">
+        <v>321</v>
+      </c>
+      <c r="G180" s="20" t="s">
+        <v>317</v>
+      </c>
       <c r="H180" s="65">
         <f>IF(Table2[[#This Row],[STEPmod publication index]]=Table2[[#This Row],[Final Listing]],1,0)</f>
         <v>1</v>
@@ -23722,16 +23707,16 @@
         <v>21</v>
       </c>
       <c r="K180" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="L180" s="17" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="L180" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="M180" s="17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="N180" s="18">
-        <f t="shared" si="28"/>
+        <f t="shared" ref="N180:N188" si="28">IF(ISBLANK(E180),0,1)</f>
         <v>1</v>
       </c>
       <c r="O180" s="16"/>
@@ -23740,8 +23725,8 @@
         <v>1</v>
       </c>
       <c r="Q180" s="19">
-        <f t="shared" si="29"/>
-        <v>1</v>
+        <f t="shared" ref="Q180:Q188" si="29">IF(AND(I180="Yes",J180="CR11",K180=L180,L180=M180,M180=E180),1,IF(AND(I180="Yes",J180="CR11",K180=M180,M180=E180),0.5,0))</f>
+        <v>0</v>
       </c>
       <c r="R180" s="3"/>
       <c r="S180" s="3"/>
@@ -23752,18 +23737,18 @@
     </row>
     <row r="181" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A181" s="98">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="B181" s="16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C181" s="54">
         <v>2</v>
       </c>
-      <c r="D181" s="87" t="s">
+      <c r="D181" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E181" s="86" t="s">
+      <c r="E181" s="53" t="s">
         <v>27</v>
       </c>
       <c r="F181" s="71" t="s">
@@ -23811,13 +23796,13 @@
     </row>
     <row r="182" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A182" s="98">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="B182" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="C182" s="54" t="s">
-        <v>128</v>
+        <v>222</v>
+      </c>
+      <c r="C182" s="54">
+        <v>2</v>
       </c>
       <c r="D182" s="87" t="s">
         <v>27</v>
@@ -23828,10 +23813,8 @@
       <c r="F182" s="71" t="s">
         <v>323</v>
       </c>
-      <c r="G182" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="H182" s="94">
+      <c r="G182" s="72"/>
+      <c r="H182" s="65">
         <f>IF(Table2[[#This Row],[STEPmod publication index]]=Table2[[#This Row],[Final Listing]],1,0)</f>
         <v>1</v>
       </c>
@@ -23841,9 +23824,11 @@
       <c r="J182" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K182" s="55"/>
-      <c r="L182" s="16" t="s">
-        <v>29</v>
+      <c r="K182" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="L182" s="17" t="s">
+        <v>27</v>
       </c>
       <c r="M182" s="17" t="s">
         <v>27</v>
@@ -23854,12 +23839,12 @@
       </c>
       <c r="O182" s="16"/>
       <c r="P182" s="18">
-        <f>IF(ISBLANK(G182),IF(ISBLANK(E182),0,1),1)</f>
+        <f>IF(ISBLANK(O182),IF(ISBLANK(E182),0,1),1)</f>
         <v>1</v>
       </c>
       <c r="Q182" s="19">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R182" s="3"/>
       <c r="S182" s="3"/>
@@ -23870,25 +23855,27 @@
     </row>
     <row r="183" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A183" s="98">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="B183" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="C183" s="54">
-        <v>2</v>
-      </c>
-      <c r="D183" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="E183" s="53" t="s">
-        <v>29</v>
-      </c>
-      <c r="F183" s="86" t="s">
-        <v>322</v>
-      </c>
-      <c r="G183" s="72"/>
-      <c r="H183" s="65">
+        <v>223</v>
+      </c>
+      <c r="C183" s="54" t="s">
+        <v>128</v>
+      </c>
+      <c r="D183" s="87" t="s">
+        <v>27</v>
+      </c>
+      <c r="E183" s="86" t="s">
+        <v>27</v>
+      </c>
+      <c r="F183" s="71" t="s">
+        <v>323</v>
+      </c>
+      <c r="G183" s="73" t="s">
+        <v>128</v>
+      </c>
+      <c r="H183" s="94">
         <f>IF(Table2[[#This Row],[STEPmod publication index]]=Table2[[#This Row],[Final Listing]],1,0)</f>
         <v>1</v>
       </c>
@@ -23898,14 +23885,12 @@
       <c r="J183" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K183" s="55" t="s">
-        <v>29</v>
-      </c>
+      <c r="K183" s="55"/>
       <c r="L183" s="16" t="s">
         <v>29</v>
       </c>
       <c r="M183" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N183" s="18">
         <f t="shared" si="28"/>
@@ -23913,12 +23898,12 @@
       </c>
       <c r="O183" s="16"/>
       <c r="P183" s="18">
-        <f>IF(ISBLANK(O183),IF(ISBLANK(E183),0,1),1)</f>
+        <f>IF(ISBLANK(G183),IF(ISBLANK(E183),0,1),1)</f>
         <v>1</v>
       </c>
       <c r="Q183" s="19">
         <f t="shared" si="29"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R183" s="3"/>
       <c r="S183" s="3"/>
@@ -23929,10 +23914,10 @@
     </row>
     <row r="184" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A184" s="98">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="B184" s="16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C184" s="54">
         <v>2</v>
@@ -23988,22 +23973,22 @@
     </row>
     <row r="185" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A185" s="98">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="B185" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C185" s="54">
         <v>2</v>
       </c>
-      <c r="D185" s="56" t="s">
-        <v>19</v>
+      <c r="D185" s="31" t="s">
+        <v>29</v>
       </c>
       <c r="E185" s="53" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="F185" s="86" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G185" s="72"/>
       <c r="H185" s="65">
@@ -24017,13 +24002,13 @@
         <v>21</v>
       </c>
       <c r="K185" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="L185" s="17" t="s">
-        <v>19</v>
+        <v>29</v>
+      </c>
+      <c r="L185" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="M185" s="17" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="N185" s="18">
         <f t="shared" si="28"/>
@@ -24047,24 +24032,24 @@
     </row>
     <row r="186" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A186" s="98">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="B186" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C186" s="54">
         <v>2</v>
       </c>
-      <c r="D186" s="87" t="s">
-        <v>24</v>
-      </c>
-      <c r="E186" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="F186" s="72" t="s">
-        <v>320</v>
-      </c>
-      <c r="G186" s="20"/>
+      <c r="D186" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="E186" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="F186" s="86" t="s">
+        <v>323</v>
+      </c>
+      <c r="G186" s="72"/>
       <c r="H186" s="65">
         <f>IF(Table2[[#This Row],[STEPmod publication index]]=Table2[[#This Row],[Final Listing]],1,0)</f>
         <v>1</v>
@@ -24076,26 +24061,26 @@
         <v>21</v>
       </c>
       <c r="K186" s="55" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="L186" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="M186" s="16"/>
+        <v>19</v>
+      </c>
+      <c r="M186" s="17" t="s">
+        <v>19</v>
+      </c>
       <c r="N186" s="18">
         <f t="shared" si="28"/>
         <v>1</v>
       </c>
-      <c r="O186" s="17" t="s">
-        <v>24</v>
-      </c>
+      <c r="O186" s="16"/>
       <c r="P186" s="18">
         <f>IF(ISBLANK(O186),IF(ISBLANK(E186),0,1),1)</f>
         <v>1</v>
       </c>
       <c r="Q186" s="19">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R186" s="3"/>
       <c r="S186" s="3"/>
@@ -24106,26 +24091,24 @@
     </row>
     <row r="187" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A187" s="98">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="B187" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C187" s="54">
         <v>2</v>
       </c>
-      <c r="D187" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="E187" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="F187" s="71" t="s">
-        <v>323</v>
-      </c>
-      <c r="G187" s="72" t="s">
-        <v>318</v>
-      </c>
+      <c r="D187" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="E187" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="F187" s="72" t="s">
+        <v>320</v>
+      </c>
+      <c r="G187" s="20"/>
       <c r="H187" s="65">
         <f>IF(Table2[[#This Row],[STEPmod publication index]]=Table2[[#This Row],[Final Listing]],1,0)</f>
         <v>1</v>
@@ -24137,26 +24120,26 @@
         <v>21</v>
       </c>
       <c r="K187" s="55" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L187" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="M187" s="17" t="s">
-        <v>27</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="M187" s="16"/>
       <c r="N187" s="18">
         <f t="shared" si="28"/>
         <v>1</v>
       </c>
-      <c r="O187" s="16"/>
+      <c r="O187" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="P187" s="18">
         <f>IF(ISBLANK(O187),IF(ISBLANK(E187),0,1),1)</f>
         <v>1</v>
       </c>
       <c r="Q187" s="19">
         <f t="shared" si="29"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R187" s="3"/>
       <c r="S187" s="3"/>
@@ -24173,31 +24156,52 @@
         <v>228</v>
       </c>
       <c r="C188" s="54">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D188" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="E188" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F188" s="72" t="s">
-        <v>321</v>
-      </c>
-      <c r="G188" s="20"/>
+        <v>27</v>
+      </c>
+      <c r="E188" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F188" s="71" t="s">
+        <v>323</v>
+      </c>
+      <c r="G188" s="72" t="s">
+        <v>318</v>
+      </c>
       <c r="H188" s="65">
         <f>IF(Table2[[#This Row],[STEPmod publication index]]=Table2[[#This Row],[Final Listing]],1,0)</f>
         <v>1</v>
       </c>
-      <c r="I188" s="16"/>
-      <c r="J188" s="16"/>
-      <c r="K188" s="37"/>
-      <c r="L188" s="16"/>
-      <c r="M188" s="17"/>
-      <c r="N188" s="18"/>
+      <c r="I188" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J188" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="K188" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="L188" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="M188" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="N188" s="18">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
       <c r="O188" s="16"/>
-      <c r="P188" s="18"/>
-      <c r="Q188" s="19"/>
+      <c r="P188" s="18">
+        <f>IF(ISBLANK(O188),IF(ISBLANK(E188),0,1),1)</f>
+        <v>1</v>
+      </c>
+      <c r="Q188" s="19">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
       <c r="R188" s="3"/>
       <c r="S188" s="3"/>
       <c r="T188" s="3"/>
@@ -24207,56 +24211,37 @@
     </row>
     <row r="189" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A189" s="98">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="B189" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C189" s="54">
-        <v>2</v>
-      </c>
-      <c r="D189" s="84" t="s">
-        <v>27</v>
-      </c>
-      <c r="E189" s="86" t="s">
-        <v>27</v>
-      </c>
-      <c r="F189" s="71" t="s">
-        <v>323</v>
-      </c>
-      <c r="G189" s="72"/>
+        <v>3</v>
+      </c>
+      <c r="D189" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="E189" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F189" s="72" t="s">
+        <v>321</v>
+      </c>
+      <c r="G189" s="20"/>
       <c r="H189" s="65">
         <f>IF(Table2[[#This Row],[STEPmod publication index]]=Table2[[#This Row],[Final Listing]],1,0)</f>
         <v>1</v>
       </c>
-      <c r="I189" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J189" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="K189" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="L189" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="M189" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="N189" s="18">
-        <f t="shared" ref="N189:N204" si="30">IF(ISBLANK(E189),0,1)</f>
-        <v>1</v>
-      </c>
+      <c r="I189" s="16"/>
+      <c r="J189" s="16"/>
+      <c r="K189" s="37"/>
+      <c r="L189" s="16"/>
+      <c r="M189" s="17"/>
+      <c r="N189" s="18"/>
       <c r="O189" s="16"/>
-      <c r="P189" s="18">
-        <f t="shared" ref="P189:P200" si="31">IF(ISBLANK(O189),IF(ISBLANK(E189),0,1),1)</f>
-        <v>1</v>
-      </c>
-      <c r="Q189" s="19">
-        <f t="shared" ref="Q189:Q204" si="32">IF(AND(I189="Yes",J189="CR11",K189=L189,L189=M189,M189=E189),1,IF(AND(I189="Yes",J189="CR11",K189=M189,M189=E189),0.5,0))</f>
-        <v>1</v>
-      </c>
+      <c r="P189" s="18"/>
+      <c r="Q189" s="19"/>
       <c r="R189" s="3"/>
       <c r="S189" s="3"/>
       <c r="T189" s="3"/>
@@ -24266,19 +24251,19 @@
     </row>
     <row r="190" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A190" s="98">
-        <v>1819</v>
+        <v>1816</v>
       </c>
       <c r="B190" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C190" s="54">
         <v>2</v>
       </c>
       <c r="D190" s="84" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E190" s="86" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F190" s="71" t="s">
         <v>323</v>
@@ -24295,25 +24280,25 @@
         <v>21</v>
       </c>
       <c r="K190" s="55" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="L190" s="17" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="M190" s="17" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="N190" s="18">
-        <f t="shared" si="30"/>
+        <f t="shared" ref="N190:N205" si="30">IF(ISBLANK(E190),0,1)</f>
         <v>1</v>
       </c>
       <c r="O190" s="16"/>
       <c r="P190" s="18">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="P190:P201" si="31">IF(ISBLANK(O190),IF(ISBLANK(E190),0,1),1)</f>
         <v>1</v>
       </c>
       <c r="Q190" s="19">
-        <f t="shared" si="32"/>
+        <f t="shared" ref="Q190:Q205" si="32">IF(AND(I190="Yes",J190="CR11",K190=L190,L190=M190,M190=E190),1,IF(AND(I190="Yes",J190="CR11",K190=M190,M190=E190),0.5,0))</f>
         <v>1</v>
       </c>
       <c r="R190" s="3"/>
@@ -24325,21 +24310,21 @@
     </row>
     <row r="191" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A191" s="98">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="B191" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C191" s="54">
         <v>2</v>
       </c>
-      <c r="D191" s="56" t="s">
+      <c r="D191" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="E191" s="53" t="s">
+      <c r="E191" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="F191" s="86" t="s">
+      <c r="F191" s="71" t="s">
         <v>323</v>
       </c>
       <c r="G191" s="72"/>
@@ -24384,24 +24369,24 @@
     </row>
     <row r="192" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A192" s="98">
-        <v>1823</v>
+        <v>1820</v>
       </c>
       <c r="B192" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C192" s="54">
         <v>2</v>
       </c>
-      <c r="D192" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="E192" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="F192" s="87" t="s">
-        <v>320</v>
-      </c>
-      <c r="G192" s="20"/>
+      <c r="D192" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="E192" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="F192" s="86" t="s">
+        <v>323</v>
+      </c>
+      <c r="G192" s="72"/>
       <c r="H192" s="65">
         <f>IF(Table2[[#This Row],[STEPmod publication index]]=Table2[[#This Row],[Final Listing]],1,0)</f>
         <v>1</v>
@@ -24413,28 +24398,26 @@
         <v>21</v>
       </c>
       <c r="K192" s="55" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="L192" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="M192" s="21" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="M192" s="17" t="s">
+        <v>19</v>
       </c>
       <c r="N192" s="18">
         <f t="shared" si="30"/>
         <v>1</v>
       </c>
-      <c r="O192" s="17" t="s">
-        <v>24</v>
-      </c>
+      <c r="O192" s="16"/>
       <c r="P192" s="18">
         <f t="shared" si="31"/>
         <v>1</v>
       </c>
       <c r="Q192" s="19">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R192" s="3"/>
       <c r="S192" s="3"/>
@@ -24445,18 +24428,18 @@
     </row>
     <row r="193" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A193" s="98">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="B193" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C193" s="54">
         <v>2</v>
       </c>
-      <c r="D193" s="87" t="s">
+      <c r="D193" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E193" s="87" t="s">
+      <c r="E193" s="31" t="s">
         <v>24</v>
       </c>
       <c r="F193" s="87" t="s">
@@ -24506,22 +24489,22 @@
     </row>
     <row r="194" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A194" s="98">
-        <v>1826</v>
+        <v>1824</v>
       </c>
       <c r="B194" s="16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C194" s="54">
-        <v>1</v>
-      </c>
-      <c r="D194" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="E194" s="53" t="s">
-        <v>38</v>
+        <v>2</v>
+      </c>
+      <c r="D194" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="E194" s="87" t="s">
+        <v>24</v>
       </c>
       <c r="F194" s="87" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G194" s="20"/>
       <c r="H194" s="65">
@@ -24535,19 +24518,21 @@
         <v>21</v>
       </c>
       <c r="K194" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="L194" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="M194" s="17" t="s">
-        <v>79</v>
+        <v>24</v>
+      </c>
+      <c r="L194" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M194" s="21" t="s">
+        <v>25</v>
       </c>
       <c r="N194" s="18">
         <f t="shared" si="30"/>
         <v>1</v>
       </c>
-      <c r="O194" s="16"/>
+      <c r="O194" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="P194" s="18">
         <f t="shared" si="31"/>
         <v>1</v>
@@ -24565,10 +24550,10 @@
     </row>
     <row r="195" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A195" s="98">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="B195" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C195" s="54">
         <v>1</v>
@@ -24594,13 +24579,13 @@
         <v>21</v>
       </c>
       <c r="K195" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="L195" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="L195" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="M195" s="16" t="s">
-        <v>38</v>
+      <c r="M195" s="17" t="s">
+        <v>79</v>
       </c>
       <c r="N195" s="18">
         <f t="shared" si="30"/>
@@ -24613,7 +24598,7 @@
       </c>
       <c r="Q195" s="19">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R195" s="3"/>
       <c r="S195" s="3"/>
@@ -24624,10 +24609,10 @@
     </row>
     <row r="196" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A196" s="98">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="B196" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C196" s="54">
         <v>1</v>
@@ -24638,7 +24623,7 @@
       <c r="E196" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="F196" s="72" t="s">
+      <c r="F196" s="87" t="s">
         <v>321</v>
       </c>
       <c r="G196" s="20"/>
@@ -24655,7 +24640,7 @@
       <c r="K196" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="L196" s="17" t="s">
+      <c r="L196" s="16" t="s">
         <v>38</v>
       </c>
       <c r="M196" s="16" t="s">
@@ -24683,22 +24668,22 @@
     </row>
     <row r="197" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A197" s="98">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="B197" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C197" s="54">
         <v>1</v>
       </c>
-      <c r="D197" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="E197" s="31" t="s">
-        <v>80</v>
+      <c r="D197" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="E197" s="53" t="s">
+        <v>38</v>
       </c>
       <c r="F197" s="72" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G197" s="20"/>
       <c r="H197" s="65">
@@ -24712,13 +24697,13 @@
         <v>21</v>
       </c>
       <c r="K197" s="55" t="s">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="L197" s="17" t="s">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="M197" s="16" t="s">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="N197" s="18">
         <f t="shared" si="30"/>
@@ -24742,24 +24727,24 @@
     </row>
     <row r="198" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A198" s="98">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="B198" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C198" s="54">
         <v>1</v>
       </c>
-      <c r="D198" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="E198" s="53" t="s">
-        <v>19</v>
-      </c>
-      <c r="F198" s="71" t="s">
-        <v>323</v>
-      </c>
-      <c r="G198" s="72"/>
+      <c r="D198" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="E198" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="F198" s="72" t="s">
+        <v>320</v>
+      </c>
+      <c r="G198" s="20"/>
       <c r="H198" s="65">
         <f>IF(Table2[[#This Row],[STEPmod publication index]]=Table2[[#This Row],[Final Listing]],1,0)</f>
         <v>1</v>
@@ -24771,13 +24756,13 @@
         <v>21</v>
       </c>
       <c r="K198" s="55" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="L198" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="M198" s="17" t="s">
-        <v>19</v>
+        <v>80</v>
+      </c>
+      <c r="M198" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="N198" s="18">
         <f t="shared" si="30"/>
@@ -24801,10 +24786,10 @@
     </row>
     <row r="199" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A199" s="98">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="B199" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C199" s="54">
         <v>1</v>
@@ -24859,37 +24844,43 @@
       <c r="Y199" s="3"/>
     </row>
     <row r="200" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A200" s="97">
-        <v>1834</v>
+      <c r="A200" s="98">
+        <v>1831</v>
       </c>
       <c r="B200" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C200" s="54">
         <v>1</v>
       </c>
-      <c r="D200" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="E200" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F200" s="87" t="s">
-        <v>321</v>
-      </c>
-      <c r="G200" s="20"/>
+      <c r="D200" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="E200" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="F200" s="71" t="s">
+        <v>323</v>
+      </c>
+      <c r="G200" s="72"/>
       <c r="H200" s="65">
         <f>IF(Table2[[#This Row],[STEPmod publication index]]=Table2[[#This Row],[Final Listing]],1,0)</f>
         <v>1</v>
       </c>
-      <c r="I200" s="16"/>
-      <c r="J200" s="16"/>
+      <c r="I200" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J200" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="K200" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="L200" s="16"/>
-      <c r="M200" s="16" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="L200" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="M200" s="17" t="s">
+        <v>19</v>
       </c>
       <c r="N200" s="18">
         <f t="shared" si="30"/>
@@ -24902,7 +24893,7 @@
       </c>
       <c r="Q200" s="19">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R200" s="3"/>
       <c r="S200" s="3"/>
@@ -24912,41 +24903,45 @@
       <c r="Y200" s="3"/>
     </row>
     <row r="201" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A201" s="26">
-        <v>1835</v>
-      </c>
-      <c r="B201" s="80" t="s">
-        <v>325</v>
-      </c>
-      <c r="C201" s="83">
-        <v>1</v>
-      </c>
-      <c r="D201" s="80"/>
-      <c r="E201" s="80"/>
+      <c r="A201" s="97">
+        <v>1834</v>
+      </c>
+      <c r="B201" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="C201" s="54">
+        <v>1</v>
+      </c>
+      <c r="D201" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E201" s="31" t="s">
+        <v>17</v>
+      </c>
       <c r="F201" s="87" t="s">
         <v>321</v>
       </c>
-      <c r="G201" s="20" t="s">
-        <v>326</v>
-      </c>
+      <c r="G201" s="20"/>
       <c r="H201" s="65">
         <f>IF(Table2[[#This Row],[STEPmod publication index]]=Table2[[#This Row],[Final Listing]],1,0)</f>
         <v>1</v>
       </c>
       <c r="I201" s="16"/>
       <c r="J201" s="16"/>
-      <c r="K201" s="16"/>
+      <c r="K201" s="55" t="s">
+        <v>17</v>
+      </c>
       <c r="L201" s="16"/>
-      <c r="M201" s="17" t="s">
-        <v>62</v>
+      <c r="M201" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="N201" s="18">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O201" s="16"/>
       <c r="P201" s="18">
-        <f>IF(ISBLANK(G201),IF(ISBLANK(E201),0,1),1)</f>
+        <f t="shared" si="31"/>
         <v>1</v>
       </c>
       <c r="Q201" s="19">
@@ -24961,45 +24956,41 @@
       <c r="Y201" s="3"/>
     </row>
     <row r="202" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A202" s="97">
-        <v>1836</v>
-      </c>
-      <c r="B202" s="16" t="s">
-        <v>242</v>
-      </c>
-      <c r="C202" s="54">
-        <v>1</v>
-      </c>
-      <c r="D202" s="87" t="s">
-        <v>17</v>
-      </c>
-      <c r="E202" s="87" t="s">
-        <v>17</v>
-      </c>
+      <c r="A202" s="26">
+        <v>1835</v>
+      </c>
+      <c r="B202" s="80" t="s">
+        <v>325</v>
+      </c>
+      <c r="C202" s="83">
+        <v>1</v>
+      </c>
+      <c r="D202" s="80"/>
+      <c r="E202" s="80"/>
       <c r="F202" s="87" t="s">
         <v>321</v>
       </c>
-      <c r="G202" s="20"/>
+      <c r="G202" s="20" t="s">
+        <v>326</v>
+      </c>
       <c r="H202" s="65">
         <f>IF(Table2[[#This Row],[STEPmod publication index]]=Table2[[#This Row],[Final Listing]],1,0)</f>
         <v>1</v>
       </c>
       <c r="I202" s="16"/>
       <c r="J202" s="16"/>
-      <c r="K202" s="55" t="s">
-        <v>17</v>
-      </c>
+      <c r="K202" s="16"/>
       <c r="L202" s="16"/>
-      <c r="M202" s="16" t="s">
-        <v>17</v>
+      <c r="M202" s="17" t="s">
+        <v>62</v>
       </c>
       <c r="N202" s="18">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O202" s="16"/>
       <c r="P202" s="18">
-        <f>IF(ISBLANK(O202),IF(ISBLANK(E202),0,1),1)</f>
+        <f>IF(ISBLANK(G202),IF(ISBLANK(E202),0,1),1)</f>
         <v>1</v>
       </c>
       <c r="Q202" s="19">
@@ -25014,43 +25005,43 @@
       <c r="Y202" s="3"/>
     </row>
     <row r="203" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A203" s="26">
-        <v>1844</v>
+      <c r="A203" s="97">
+        <v>1836</v>
       </c>
       <c r="B203" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="C203" s="19">
-        <v>1</v>
-      </c>
-      <c r="D203" s="84" t="s">
-        <v>38</v>
-      </c>
-      <c r="E203" s="86" t="s">
-        <v>38</v>
-      </c>
-      <c r="F203" s="72" t="s">
+        <v>242</v>
+      </c>
+      <c r="C203" s="54">
+        <v>1</v>
+      </c>
+      <c r="D203" s="87" t="s">
+        <v>17</v>
+      </c>
+      <c r="E203" s="87" t="s">
+        <v>17</v>
+      </c>
+      <c r="F203" s="87" t="s">
         <v>321</v>
       </c>
-      <c r="G203" s="20" t="s">
-        <v>319</v>
-      </c>
+      <c r="G203" s="20"/>
       <c r="H203" s="65">
         <f>IF(Table2[[#This Row],[STEPmod publication index]]=Table2[[#This Row],[Final Listing]],1,0)</f>
         <v>1</v>
       </c>
       <c r="I203" s="16"/>
       <c r="J203" s="16"/>
-      <c r="K203" s="16"/>
+      <c r="K203" s="55" t="s">
+        <v>17</v>
+      </c>
       <c r="L203" s="16"/>
-      <c r="M203" s="16"/>
+      <c r="M203" s="16" t="s">
+        <v>17</v>
+      </c>
       <c r="N203" s="18">
         <f t="shared" si="30"/>
         <v>1</v>
       </c>
-      <c r="O203" s="17" t="s">
-        <v>38</v>
-      </c>
+      <c r="O203" s="16"/>
       <c r="P203" s="18">
         <f>IF(ISBLANK(O203),IF(ISBLANK(E203),0,1),1)</f>
         <v>1</v>
@@ -25067,22 +25058,22 @@
       <c r="Y203" s="3"/>
     </row>
     <row r="204" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A204" s="97">
-        <v>1845</v>
-      </c>
-      <c r="B204" s="81" t="s">
-        <v>244</v>
-      </c>
-      <c r="C204" s="74">
-        <v>1</v>
-      </c>
-      <c r="D204" s="100" t="s">
+      <c r="A204" s="26">
+        <v>1844</v>
+      </c>
+      <c r="B204" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="C204" s="19">
+        <v>1</v>
+      </c>
+      <c r="D204" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="E204" s="101" t="s">
+      <c r="E204" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="F204" s="87" t="s">
+      <c r="F204" s="72" t="s">
         <v>321</v>
       </c>
       <c r="G204" s="20" t="s">
@@ -25119,95 +25110,148 @@
       <c r="X204" s="3"/>
       <c r="Y204" s="3"/>
     </row>
-    <row r="205" spans="1:25" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A205" s="69" t="s">
-        <v>69</v>
-      </c>
-      <c r="B205" s="77" t="s">
-        <v>68</v>
-      </c>
-      <c r="C205" s="63">
-        <v>1</v>
-      </c>
-      <c r="D205" s="31"/>
-      <c r="E205" s="31"/>
-      <c r="F205" s="72" t="s">
+    <row r="205" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A205" s="97">
+        <v>1845</v>
+      </c>
+      <c r="B205" s="81" t="s">
+        <v>244</v>
+      </c>
+      <c r="C205" s="74">
+        <v>1</v>
+      </c>
+      <c r="D205" s="100" t="s">
+        <v>38</v>
+      </c>
+      <c r="E205" s="101" t="s">
+        <v>38</v>
+      </c>
+      <c r="F205" s="87" t="s">
         <v>321</v>
       </c>
-      <c r="G205" s="20"/>
+      <c r="G205" s="20" t="s">
+        <v>319</v>
+      </c>
       <c r="H205" s="65">
         <f>IF(Table2[[#This Row],[STEPmod publication index]]=Table2[[#This Row],[Final Listing]],1,0)</f>
         <v>1</v>
       </c>
       <c r="I205" s="16"/>
       <c r="J205" s="16"/>
-      <c r="K205" s="37"/>
+      <c r="K205" s="16"/>
       <c r="L205" s="16"/>
-      <c r="M205" s="21"/>
-      <c r="N205" s="18"/>
-      <c r="O205" s="17"/>
-      <c r="P205" s="18"/>
-      <c r="Q205" s="19"/>
-    </row>
-    <row r="206" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A206" s="43" t="s">
+      <c r="M205" s="16"/>
+      <c r="N205" s="18">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="O205" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="P205" s="18">
+        <f>IF(ISBLANK(O205),IF(ISBLANK(E205),0,1),1)</f>
+        <v>1</v>
+      </c>
+      <c r="Q205" s="19">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="R205" s="3"/>
+      <c r="S205" s="3"/>
+      <c r="T205" s="3"/>
+      <c r="U205" s="3"/>
+      <c r="X205" s="3"/>
+      <c r="Y205" s="3"/>
+    </row>
+    <row r="206" spans="1:25" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A206" s="69" t="s">
+        <v>69</v>
+      </c>
+      <c r="B206" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="C206" s="63">
+        <v>1</v>
+      </c>
+      <c r="D206" s="31"/>
+      <c r="E206" s="31"/>
+      <c r="F206" s="72" t="s">
+        <v>321</v>
+      </c>
+      <c r="G206" s="20"/>
+      <c r="H206" s="65">
+        <f>IF(Table2[[#This Row],[STEPmod publication index]]=Table2[[#This Row],[Final Listing]],1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I206" s="16"/>
+      <c r="J206" s="16"/>
+      <c r="K206" s="37"/>
+      <c r="L206" s="16"/>
+      <c r="M206" s="21"/>
+      <c r="N206" s="18"/>
+      <c r="O206" s="17"/>
+      <c r="P206" s="18"/>
+      <c r="Q206" s="19"/>
+    </row>
+    <row r="207" spans="1:25" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A207" s="43" t="s">
         <v>263</v>
       </c>
-      <c r="B206" s="79" t="s">
+      <c r="B207" s="79" t="s">
         <v>264</v>
       </c>
-      <c r="C206" s="82">
-        <f>COUNTBLANK(C205:C205)</f>
+      <c r="C207" s="82">
+        <f>COUNTBLANK(C206:C206)</f>
         <v>0</v>
       </c>
-      <c r="D206" s="85">
-        <f>COUNTBLANK(D205:D205)</f>
-        <v>1</v>
-      </c>
-      <c r="E206" s="85">
-        <f>COUNTBLANK(E205:E205)</f>
-        <v>1</v>
-      </c>
-      <c r="F206" s="89"/>
-      <c r="G206" s="91"/>
-      <c r="H206" s="93"/>
-      <c r="I206" s="35">
-        <f>COUNTBLANK(I205:I205)</f>
-        <v>1</v>
-      </c>
-      <c r="J206" s="35">
-        <f>COUNTBLANK(J205:J205)</f>
-        <v>1</v>
-      </c>
-      <c r="K206" s="35">
-        <f>COUNTBLANK(K205:K205)</f>
-        <v>1</v>
-      </c>
-      <c r="L206" s="35">
-        <f>COUNTBLANK(L205:L205)</f>
-        <v>1</v>
-      </c>
-      <c r="M206" s="35">
-        <f>COUNTBLANK(M205:M205)</f>
-        <v>1</v>
-      </c>
-      <c r="N206" s="34"/>
-      <c r="O206" s="35"/>
-      <c r="P206" s="34"/>
-      <c r="Q206" s="34"/>
-      <c r="R206" s="3"/>
-      <c r="S206" s="3"/>
-      <c r="T206" s="3"/>
-      <c r="U206" s="3"/>
-      <c r="X206" s="3"/>
-      <c r="Y206" s="3"/>
+      <c r="D207" s="85">
+        <f>COUNTBLANK(D206:D206)</f>
+        <v>1</v>
+      </c>
+      <c r="E207" s="85">
+        <f>COUNTBLANK(E206:E206)</f>
+        <v>1</v>
+      </c>
+      <c r="F207" s="89"/>
+      <c r="G207" s="91"/>
+      <c r="H207" s="93"/>
+      <c r="I207" s="35">
+        <f>COUNTBLANK(I206:I206)</f>
+        <v>1</v>
+      </c>
+      <c r="J207" s="35">
+        <f>COUNTBLANK(J206:J206)</f>
+        <v>1</v>
+      </c>
+      <c r="K207" s="35">
+        <f>COUNTBLANK(K206:K206)</f>
+        <v>1</v>
+      </c>
+      <c r="L207" s="35">
+        <f>COUNTBLANK(L206:L206)</f>
+        <v>1</v>
+      </c>
+      <c r="M207" s="35">
+        <f>COUNTBLANK(M206:M206)</f>
+        <v>1</v>
+      </c>
+      <c r="N207" s="34"/>
+      <c r="O207" s="35"/>
+      <c r="P207" s="34"/>
+      <c r="Q207" s="34"/>
+      <c r="R207" s="3"/>
+      <c r="S207" s="3"/>
+      <c r="T207" s="3"/>
+      <c r="U207" s="3"/>
+      <c r="X207" s="3"/>
+      <c r="Y207" s="3"/>
     </row>
   </sheetData>
   <sortState ref="A2:T196">
     <sortCondition ref="A2:A196"/>
   </sortState>
   <phoneticPr fontId="12" type="noConversion"/>
-  <conditionalFormatting sqref="T207:T1048576 Q1 N66:N196 N1:N4 Y207:Y1048576 Q76:Q196 Q198 N198 N200:N206 Q200:Q206 N6:N64">
+  <conditionalFormatting sqref="T208:T1048576 Q1 N66:N197 N1:N4 Y208:Y1048576 Q76:Q197 Q199 N199 N201:N207 Q201:Q207 N6:N64">
     <cfRule type="iconSet" priority="20">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -25216,7 +25260,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X207:X1048576 P1:P4 P66:P196 P198 P200:P206 P6:P64">
+  <conditionalFormatting sqref="X208:X1048576 P1:P4 P66:P197 P199 P201:P207 P6:P64">
     <cfRule type="iconSet" priority="18">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -25306,7 +25350,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N197 Q197">
+  <conditionalFormatting sqref="N198 Q198">
     <cfRule type="iconSet" priority="5">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -25315,7 +25359,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P197">
+  <conditionalFormatting sqref="P198">
     <cfRule type="iconSet" priority="4">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -25324,7 +25368,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q199 N199">
+  <conditionalFormatting sqref="Q200 N200">
     <cfRule type="iconSet" priority="3">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -25333,7 +25377,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P199">
+  <conditionalFormatting sqref="P200">
     <cfRule type="iconSet" priority="2">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>

</xml_diff>